<commit_message>
added GPLv3 to the project; fixed some Analyser template issues.
</commit_message>
<xml_diff>
--- a/SolarLoadModel/Data/Analyser.xlsx
+++ b/SolarLoadModel/Data/Analyser.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="28830" windowHeight="12795" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="105" windowWidth="20730" windowHeight="11700" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Gen Running Costs" sheetId="1" r:id="rId1"/>
@@ -1423,7 +1423,7 @@
     <row r="2" spans="1:21" s="7" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
         <f>CONCATENATE("Approximate Run Time: ", Leftover_Years_Run, " year(s) ", Leftover_Months_Run, " month(s) ", Leftover_Days_Run, " day(s)")</f>
-        <v>Approximate Run Time: 1 year(s) 10 month(s) 26 day(s)</v>
+        <v>Approximate Run Time: 1 year(s) 10 month(s) 21 day(s)</v>
       </c>
       <c r="F2" s="33"/>
       <c r="G2" s="33"/>
@@ -2460,8 +2460,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AR95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2489,7 +2489,7 @@
         <v>125</v>
       </c>
       <c r="B3" s="48">
-        <f>autofill!A2-(autofill!A3-autofill!A2)+1+TIME(0,0,1)</f>
+        <f>autofill!A2</f>
         <v>25569</v>
       </c>
       <c r="C3" s="31"/>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="B4" s="48">
         <f>INDEX(autofill!$A:$A, COUNTA(autofill!$A:$A), 1)</f>
-        <v>26260.999988425927</v>
+        <v>26254.999988425927</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -2525,8 +2525,8 @@
         <v>33</v>
       </c>
       <c r="B6" s="9">
-        <f>Total_Minutes*60</f>
-        <v>59788799.000000082</v>
+        <f>(Finished_On-Started_On)*86400+1</f>
+        <v>59270400.000000082</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2534,8 +2534,8 @@
         <v>34</v>
       </c>
       <c r="B7" s="9">
-        <f>Total_Hours*60</f>
-        <v>996479.98333333468</v>
+        <f>Total_Seconds/60</f>
+        <v>987840.0000000014</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2543,8 +2543,8 @@
         <v>35</v>
       </c>
       <c r="B8" s="9">
-        <f>Total_Days*24</f>
-        <v>16607.999722222245</v>
+        <f>Total_Minutes/60</f>
+        <v>16464.000000000022</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2552,8 +2552,8 @@
         <v>36</v>
       </c>
       <c r="B9" s="9">
-        <f>Finished_On-Started_On</f>
-        <v>691.99998842592686</v>
+        <f>Total_Hours/24</f>
+        <v>686.00000000000091</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B10" s="9">
         <f>Total_Days/7</f>
-        <v>98.857141203703833</v>
+        <v>98.000000000000128</v>
       </c>
       <c r="E10" s="49"/>
       <c r="F10" s="49"/>
@@ -2573,7 +2573,7 @@
       </c>
       <c r="B11" s="9">
         <f>Total_Days/30</f>
-        <v>23.066666280864229</v>
+        <v>22.866666666666696</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="B12" s="9">
         <f>YEARFRAC(Started_On,Finished_On,1)</f>
-        <v>1.893150684931507</v>
+        <v>1.8767123287671232</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
@@ -2621,7 +2621,7 @@
       </c>
       <c r="B16">
         <f>ROUNDDOWN((Total_Seconds-(Leftover_Months_Run*Seconds_in_a_Month__30d+Leftover_Years_Run*Seconds_in_a_Year))/Seconds_in_a_day,0)</f>
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C16" s="31"/>
       <c r="D16" s="31"/>
@@ -2636,7 +2636,7 @@
       </c>
       <c r="B17" s="31">
         <f>ROUNDDOWN((Total_Seconds-(Leftover_Years_Run*Seconds_in_a_Year+Leftover_Months_Run*Seconds_in_a_Month__30d+Leftover_Days_Run*Seconds_in_a_day))/Seconds_in_an_hour,0)</f>
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="C17" s="31"/>
       <c r="D17" s="31"/>
@@ -2955,11 +2955,11 @@
       </c>
       <c r="E30" s="31">
         <f>Y30</f>
-        <v>8734.9836111111108</v>
+        <v>8902.9836111111108</v>
       </c>
       <c r="F30" s="31">
         <f>MAX(Z30-Y30,0)</f>
-        <v>7896</v>
+        <v>7728</v>
       </c>
       <c r="G30" s="31">
         <f t="shared" ref="G30:X30" si="0">MAX(AA30-Z30,0)</f>
@@ -3035,7 +3035,7 @@
       </c>
       <c r="Y30" s="31">
         <f>DMAX(autofill!$1:$1048576,$A30,RangeYear1)</f>
-        <v>8734.9836111111108</v>
+        <v>8902.9836111111108</v>
       </c>
       <c r="Z30" s="31">
         <f>DMAX(autofill!$1:$1048576,$A30,RangeYear2)</f>
@@ -3131,11 +3131,11 @@
       </c>
       <c r="E31" s="31">
         <f t="shared" ref="E31:E53" si="1">Y31</f>
-        <v>8717.0774999999994</v>
+        <v>8885.0774999999994</v>
       </c>
       <c r="F31" s="31">
         <f t="shared" ref="F31:F53" si="2">MAX(Z31-Y31,0)</f>
-        <v>7896</v>
+        <v>7728</v>
       </c>
       <c r="G31" s="31">
         <f t="shared" ref="G31:G53" si="3">MAX(AA31-Z31,0)</f>
@@ -3211,7 +3211,7 @@
       </c>
       <c r="Y31" s="31">
         <f>DMAX(autofill!$1:$1048576,$A31,RangeYear1)</f>
-        <v>8717.0774999999994</v>
+        <v>8885.0774999999994</v>
       </c>
       <c r="Z31" s="31">
         <f>DMAX(autofill!$1:$1048576,$A31,RangeYear2)</f>
@@ -3307,11 +3307,11 @@
       </c>
       <c r="E32" s="31">
         <f t="shared" si="1"/>
-        <v>8689.7938888888893</v>
+        <v>8857.7938888888893</v>
       </c>
       <c r="F32" s="31">
         <f t="shared" si="2"/>
-        <v>7896</v>
+        <v>7728</v>
       </c>
       <c r="G32" s="31">
         <f t="shared" si="3"/>
@@ -3387,7 +3387,7 @@
       </c>
       <c r="Y32" s="31">
         <f>DMAX(autofill!$1:$1048576,$A32,RangeYear1)</f>
-        <v>8689.7938888888893</v>
+        <v>8857.7938888888893</v>
       </c>
       <c r="Z32" s="31">
         <f>DMAX(autofill!$1:$1048576,$A32,RangeYear2)</f>
@@ -4363,11 +4363,11 @@
       </c>
       <c r="E38" s="31">
         <f t="shared" si="1"/>
-        <v>520</v>
+        <v>530</v>
       </c>
       <c r="F38" s="31">
         <f t="shared" si="2"/>
-        <v>470</v>
+        <v>460</v>
       </c>
       <c r="G38" s="31">
         <f t="shared" si="3"/>
@@ -4443,7 +4443,7 @@
       </c>
       <c r="Y38" s="31">
         <f>DMAX(autofill!$1:$1048576,$A38,RangeYear1)</f>
-        <v>520</v>
+        <v>530</v>
       </c>
       <c r="Z38" s="31">
         <f>DMAX(autofill!$1:$1048576,$A38,RangeYear2)</f>
@@ -4539,11 +4539,11 @@
       </c>
       <c r="E39" s="31">
         <f t="shared" si="1"/>
-        <v>416</v>
+        <v>424</v>
       </c>
       <c r="F39" s="31">
         <f t="shared" si="2"/>
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="G39" s="31">
         <f t="shared" si="3"/>
@@ -4619,7 +4619,7 @@
       </c>
       <c r="Y39" s="31">
         <f>DMAX(autofill!$1:$1048576,$A39,RangeYear1)</f>
-        <v>416</v>
+        <v>424</v>
       </c>
       <c r="Z39" s="31">
         <f>DMAX(autofill!$1:$1048576,$A39,RangeYear2)</f>
@@ -4715,11 +4715,11 @@
       </c>
       <c r="E40" s="31">
         <f t="shared" si="1"/>
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="F40" s="31">
         <f t="shared" si="2"/>
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="G40" s="31">
         <f t="shared" si="3"/>
@@ -4795,7 +4795,7 @@
       </c>
       <c r="Y40" s="31">
         <f>DMAX(autofill!$1:$1048576,$A40,RangeYear1)</f>
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="Z40" s="31">
         <f>DMAX(autofill!$1:$1048576,$A40,RangeYear2)</f>
@@ -4891,11 +4891,11 @@
       </c>
       <c r="E41" s="31">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F41" s="31">
         <f t="shared" si="2"/>
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G41" s="31">
         <f t="shared" si="3"/>
@@ -4971,7 +4971,7 @@
       </c>
       <c r="Y41" s="31">
         <f>DMAX(autofill!$1:$1048576,$A41,RangeYear1)</f>
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Z41" s="31">
         <f>DMAX(autofill!$1:$1048576,$A41,RangeYear2)</f>
@@ -5067,11 +5067,11 @@
       </c>
       <c r="E42" s="31">
         <f t="shared" si="1"/>
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F42" s="31">
         <f t="shared" si="2"/>
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G42" s="31">
         <f t="shared" si="3"/>
@@ -5147,7 +5147,7 @@
       </c>
       <c r="Y42" s="31">
         <f>DMAX(autofill!$1:$1048576,$A42,RangeYear1)</f>
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="Z42" s="31">
         <f>DMAX(autofill!$1:$1048576,$A42,RangeYear2)</f>
@@ -5771,11 +5771,11 @@
       </c>
       <c r="E46" s="31">
         <f t="shared" si="1"/>
-        <v>157109.35417757501</v>
+        <v>160133.35417709101</v>
       </c>
       <c r="F46" s="31">
         <f t="shared" si="2"/>
-        <v>142127.99997725102</v>
+        <v>139103.99997773502</v>
       </c>
       <c r="G46" s="31">
         <f t="shared" si="3"/>
@@ -5851,7 +5851,7 @@
       </c>
       <c r="Y46" s="31">
         <f>DMAX(autofill!$1:$1048576,$A46,RangeYear1)</f>
-        <v>157109.35417757501</v>
+        <v>160133.35417709101</v>
       </c>
       <c r="Z46" s="31">
         <f>DMAX(autofill!$1:$1048576,$A46,RangeYear2)</f>
@@ -5947,11 +5947,11 @@
       </c>
       <c r="E47" s="31">
         <f t="shared" si="1"/>
-        <v>156801.556875621</v>
+        <v>159825.556875137</v>
       </c>
       <c r="F47" s="31">
         <f t="shared" si="2"/>
-        <v>142127.999977247</v>
+        <v>139103.999977731</v>
       </c>
       <c r="G47" s="31">
         <f t="shared" si="3"/>
@@ -6027,7 +6027,7 @@
       </c>
       <c r="Y47" s="31">
         <f>DMAX(autofill!$1:$1048576,$A47,RangeYear1)</f>
-        <v>156801.556875621</v>
+        <v>159825.556875137</v>
       </c>
       <c r="Z47" s="31">
         <f>DMAX(autofill!$1:$1048576,$A47,RangeYear2)</f>
@@ -6123,11 +6123,11 @@
       </c>
       <c r="E48" s="31">
         <f t="shared" si="1"/>
-        <v>156373.97080162301</v>
+        <v>159397.970801138</v>
       </c>
       <c r="F48" s="31">
         <f t="shared" si="2"/>
-        <v>142127.99997724697</v>
+        <v>139103.99997773199</v>
       </c>
       <c r="G48" s="31">
         <f t="shared" si="3"/>
@@ -6203,7 +6203,7 @@
       </c>
       <c r="Y48" s="31">
         <f>DMAX(autofill!$1:$1048576,$A48,RangeYear1)</f>
-        <v>156373.97080162301</v>
+        <v>159397.970801138</v>
       </c>
       <c r="Z48" s="31">
         <f>DMAX(autofill!$1:$1048576,$A48,RangeYear2)</f>
@@ -7710,7 +7710,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AC102"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7804,7 +7806,7 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="48">
-        <v>25574.999988425927</v>
+        <v>25569</v>
       </c>
       <c r="B2" s="6">
         <v>166.98361111111112</v>
@@ -7887,8 +7889,8 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="48">
-        <f>A2+7</f>
-        <v>25581.999988425927</v>
+        <f>A2+7-(1/86400)</f>
+        <v>25575.999988425927</v>
       </c>
       <c r="B3" s="6">
         <v>334.98361111111109</v>
@@ -7972,7 +7974,7 @@
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="48">
         <f t="shared" ref="A4:A67" si="0">A3+7</f>
-        <v>25588.999988425927</v>
+        <v>25582.999988425927</v>
       </c>
       <c r="B4" s="6">
         <v>502.98361111111109</v>
@@ -8056,7 +8058,7 @@
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="48">
         <f t="shared" si="0"/>
-        <v>25595.999988425927</v>
+        <v>25589.999988425927</v>
       </c>
       <c r="B5" s="6">
         <v>670.98361111111114</v>
@@ -8140,7 +8142,7 @@
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="48">
         <f t="shared" si="0"/>
-        <v>25602.999988425927</v>
+        <v>25596.999988425927</v>
       </c>
       <c r="B6" s="6">
         <v>838.98361111111114</v>
@@ -8224,7 +8226,7 @@
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="48">
         <f t="shared" si="0"/>
-        <v>25609.999988425927</v>
+        <v>25603.999988425927</v>
       </c>
       <c r="B7" s="6">
         <v>1006.9836111111111</v>
@@ -8308,7 +8310,7 @@
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="48">
         <f t="shared" si="0"/>
-        <v>25616.999988425927</v>
+        <v>25610.999988425927</v>
       </c>
       <c r="B8" s="6">
         <v>1174.983611111111</v>
@@ -8392,7 +8394,7 @@
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="48">
         <f t="shared" si="0"/>
-        <v>25623.999988425927</v>
+        <v>25617.999988425927</v>
       </c>
       <c r="B9" s="6">
         <v>1342.983611111111</v>
@@ -8476,7 +8478,7 @@
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="48">
         <f t="shared" si="0"/>
-        <v>25630.999988425927</v>
+        <v>25624.999988425927</v>
       </c>
       <c r="B10" s="6">
         <v>1510.983611111111</v>
@@ -8560,7 +8562,7 @@
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="48">
         <f t="shared" si="0"/>
-        <v>25637.999988425927</v>
+        <v>25631.999988425927</v>
       </c>
       <c r="B11" s="6">
         <v>1678.983611111111</v>
@@ -8644,7 +8646,7 @@
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="48">
         <f t="shared" si="0"/>
-        <v>25644.999988425927</v>
+        <v>25638.999988425927</v>
       </c>
       <c r="B12" s="6">
         <v>1846.983611111111</v>
@@ -8728,7 +8730,7 @@
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="48">
         <f t="shared" si="0"/>
-        <v>25651.999988425927</v>
+        <v>25645.999988425927</v>
       </c>
       <c r="B13" s="6">
         <v>2014.983611111111</v>
@@ -8812,7 +8814,7 @@
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="48">
         <f t="shared" si="0"/>
-        <v>25658.999988425927</v>
+        <v>25652.999988425927</v>
       </c>
       <c r="B14" s="6">
         <v>2182.9836111111113</v>
@@ -8896,7 +8898,7 @@
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="48">
         <f t="shared" si="0"/>
-        <v>25665.999988425927</v>
+        <v>25659.999988425927</v>
       </c>
       <c r="B15" s="6">
         <v>2350.9836111111113</v>
@@ -8980,7 +8982,7 @@
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="48">
         <f t="shared" si="0"/>
-        <v>25672.999988425927</v>
+        <v>25666.999988425927</v>
       </c>
       <c r="B16" s="6">
         <v>2518.9836111111113</v>
@@ -9064,7 +9066,7 @@
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="48">
         <f t="shared" si="0"/>
-        <v>25679.999988425927</v>
+        <v>25673.999988425927</v>
       </c>
       <c r="B17" s="6">
         <v>2686.9836111111113</v>
@@ -9148,7 +9150,7 @@
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="48">
         <f t="shared" si="0"/>
-        <v>25686.999988425927</v>
+        <v>25680.999988425927</v>
       </c>
       <c r="B18" s="6">
         <v>2854.9836111111113</v>
@@ -9232,7 +9234,7 @@
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="48">
         <f t="shared" si="0"/>
-        <v>25693.999988425927</v>
+        <v>25687.999988425927</v>
       </c>
       <c r="B19" s="6">
         <v>3022.9836111111113</v>
@@ -9316,7 +9318,7 @@
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="48">
         <f t="shared" si="0"/>
-        <v>25700.999988425927</v>
+        <v>25694.999988425927</v>
       </c>
       <c r="B20" s="6">
         <v>3190.9836111111113</v>
@@ -9400,7 +9402,7 @@
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="48">
         <f t="shared" si="0"/>
-        <v>25707.999988425927</v>
+        <v>25701.999988425927</v>
       </c>
       <c r="B21" s="6">
         <v>3358.9836111111113</v>
@@ -9484,7 +9486,7 @@
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="48">
         <f t="shared" si="0"/>
-        <v>25714.999988425927</v>
+        <v>25708.999988425927</v>
       </c>
       <c r="B22" s="6">
         <v>3526.9836111111113</v>
@@ -9568,7 +9570,7 @@
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="48">
         <f t="shared" si="0"/>
-        <v>25721.999988425927</v>
+        <v>25715.999988425927</v>
       </c>
       <c r="B23" s="6">
         <v>3694.9836111111113</v>
@@ -9652,7 +9654,7 @@
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="48">
         <f t="shared" si="0"/>
-        <v>25728.999988425927</v>
+        <v>25722.999988425927</v>
       </c>
       <c r="B24" s="6">
         <v>3862.9836111111113</v>
@@ -9736,7 +9738,7 @@
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="48">
         <f t="shared" si="0"/>
-        <v>25735.999988425927</v>
+        <v>25729.999988425927</v>
       </c>
       <c r="B25" s="6">
         <v>4030.9836111111113</v>
@@ -9820,7 +9822,7 @@
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="48">
         <f t="shared" si="0"/>
-        <v>25742.999988425927</v>
+        <v>25736.999988425927</v>
       </c>
       <c r="B26" s="6">
         <v>4198.9836111111108</v>
@@ -9904,7 +9906,7 @@
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="48">
         <f t="shared" si="0"/>
-        <v>25749.999988425927</v>
+        <v>25743.999988425927</v>
       </c>
       <c r="B27" s="6">
         <v>4366.9836111111108</v>
@@ -9988,7 +9990,7 @@
     <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="48">
         <f t="shared" si="0"/>
-        <v>25756.999988425927</v>
+        <v>25750.999988425927</v>
       </c>
       <c r="B28" s="6">
         <v>4534.9836111111108</v>
@@ -10072,7 +10074,7 @@
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="48">
         <f t="shared" si="0"/>
-        <v>25763.999988425927</v>
+        <v>25757.999988425927</v>
       </c>
       <c r="B29" s="6">
         <v>4702.9836111111108</v>
@@ -10156,7 +10158,7 @@
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="48">
         <f t="shared" si="0"/>
-        <v>25770.999988425927</v>
+        <v>25764.999988425927</v>
       </c>
       <c r="B30" s="6">
         <v>4870.9836111111108</v>
@@ -10240,7 +10242,7 @@
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="48">
         <f t="shared" si="0"/>
-        <v>25777.999988425927</v>
+        <v>25771.999988425927</v>
       </c>
       <c r="B31" s="6">
         <v>5038.9836111111108</v>
@@ -10324,7 +10326,7 @@
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="48">
         <f t="shared" si="0"/>
-        <v>25784.999988425927</v>
+        <v>25778.999988425927</v>
       </c>
       <c r="B32" s="6">
         <v>5206.9836111111108</v>
@@ -10408,7 +10410,7 @@
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="48">
         <f t="shared" si="0"/>
-        <v>25791.999988425927</v>
+        <v>25785.999988425927</v>
       </c>
       <c r="B33" s="6">
         <v>5374.9836111111108</v>
@@ -10492,7 +10494,7 @@
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="48">
         <f t="shared" si="0"/>
-        <v>25798.999988425927</v>
+        <v>25792.999988425927</v>
       </c>
       <c r="B34" s="6">
         <v>5542.9836111111108</v>
@@ -10576,7 +10578,7 @@
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="48">
         <f t="shared" si="0"/>
-        <v>25805.999988425927</v>
+        <v>25799.999988425927</v>
       </c>
       <c r="B35" s="6">
         <v>5710.9836111111108</v>
@@ -10660,7 +10662,7 @@
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="48">
         <f t="shared" si="0"/>
-        <v>25812.999988425927</v>
+        <v>25806.999988425927</v>
       </c>
       <c r="B36" s="6">
         <v>5878.9836111111108</v>
@@ -10744,7 +10746,7 @@
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="48">
         <f t="shared" si="0"/>
-        <v>25819.999988425927</v>
+        <v>25813.999988425927</v>
       </c>
       <c r="B37" s="6">
         <v>6046.9836111111108</v>
@@ -10828,7 +10830,7 @@
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="48">
         <f t="shared" si="0"/>
-        <v>25826.999988425927</v>
+        <v>25820.999988425927</v>
       </c>
       <c r="B38" s="6">
         <v>6214.9836111111108</v>
@@ -10912,7 +10914,7 @@
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="48">
         <f t="shared" si="0"/>
-        <v>25833.999988425927</v>
+        <v>25827.999988425927</v>
       </c>
       <c r="B39" s="6">
         <v>6382.9836111111108</v>
@@ -10996,7 +10998,7 @@
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="48">
         <f t="shared" si="0"/>
-        <v>25840.999988425927</v>
+        <v>25834.999988425927</v>
       </c>
       <c r="B40" s="6">
         <v>6550.9836111111108</v>
@@ -11080,7 +11082,7 @@
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="48">
         <f t="shared" si="0"/>
-        <v>25847.999988425927</v>
+        <v>25841.999988425927</v>
       </c>
       <c r="B41" s="6">
         <v>6718.9836111111108</v>
@@ -11164,7 +11166,7 @@
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="48">
         <f t="shared" si="0"/>
-        <v>25854.999988425927</v>
+        <v>25848.999988425927</v>
       </c>
       <c r="B42" s="6">
         <v>6886.9836111111108</v>
@@ -11248,7 +11250,7 @@
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="48">
         <f t="shared" si="0"/>
-        <v>25861.999988425927</v>
+        <v>25855.999988425927</v>
       </c>
       <c r="B43" s="6">
         <v>7054.9836111111108</v>
@@ -11332,7 +11334,7 @@
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="48">
         <f t="shared" si="0"/>
-        <v>25868.999988425927</v>
+        <v>25862.999988425927</v>
       </c>
       <c r="B44" s="6">
         <v>7222.9836111111108</v>
@@ -11416,7 +11418,7 @@
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="48">
         <f t="shared" si="0"/>
-        <v>25875.999988425927</v>
+        <v>25869.999988425927</v>
       </c>
       <c r="B45" s="6">
         <v>7390.9836111111108</v>
@@ -11500,7 +11502,7 @@
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" s="48">
         <f t="shared" si="0"/>
-        <v>25882.999988425927</v>
+        <v>25876.999988425927</v>
       </c>
       <c r="B46" s="6">
         <v>7558.9836111111108</v>
@@ -11584,7 +11586,7 @@
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" s="48">
         <f t="shared" si="0"/>
-        <v>25889.999988425927</v>
+        <v>25883.999988425927</v>
       </c>
       <c r="B47" s="6">
         <v>7726.9836111111108</v>
@@ -11668,7 +11670,7 @@
     <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" s="48">
         <f t="shared" si="0"/>
-        <v>25896.999988425927</v>
+        <v>25890.999988425927</v>
       </c>
       <c r="B48" s="6">
         <v>7894.9836111111108</v>
@@ -11752,7 +11754,7 @@
     <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" s="48">
         <f t="shared" si="0"/>
-        <v>25903.999988425927</v>
+        <v>25897.999988425927</v>
       </c>
       <c r="B49" s="6">
         <v>8062.9836111111108</v>
@@ -11836,7 +11838,7 @@
     <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" s="48">
         <f t="shared" si="0"/>
-        <v>25910.999988425927</v>
+        <v>25904.999988425927</v>
       </c>
       <c r="B50" s="6">
         <v>8230.9836111111108</v>
@@ -11920,7 +11922,7 @@
     <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" s="48">
         <f t="shared" si="0"/>
-        <v>25917.999988425927</v>
+        <v>25911.999988425927</v>
       </c>
       <c r="B51" s="6">
         <v>8398.9836111111108</v>
@@ -12004,7 +12006,7 @@
     <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" s="48">
         <f t="shared" si="0"/>
-        <v>25924.999988425927</v>
+        <v>25918.999988425927</v>
       </c>
       <c r="B52" s="6">
         <v>8566.9836111111108</v>
@@ -12088,7 +12090,7 @@
     <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" s="48">
         <f t="shared" si="0"/>
-        <v>25931.999988425927</v>
+        <v>25925.999988425927</v>
       </c>
       <c r="B53" s="6">
         <v>8734.9836111111108</v>
@@ -12172,7 +12174,7 @@
     <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" s="48">
         <f t="shared" si="0"/>
-        <v>25938.999988425927</v>
+        <v>25932.999988425927</v>
       </c>
       <c r="B54" s="6">
         <v>8902.9836111111108</v>
@@ -12256,7 +12258,7 @@
     <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" s="48">
         <f t="shared" si="0"/>
-        <v>25945.999988425927</v>
+        <v>25939.999988425927</v>
       </c>
       <c r="B55" s="6">
         <v>9070.9836111111108</v>
@@ -12340,7 +12342,7 @@
     <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" s="48">
         <f t="shared" si="0"/>
-        <v>25952.999988425927</v>
+        <v>25946.999988425927</v>
       </c>
       <c r="B56" s="21">
         <v>9238.9836111111108</v>
@@ -12424,7 +12426,7 @@
     <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" s="48">
         <f t="shared" si="0"/>
-        <v>25959.999988425927</v>
+        <v>25953.999988425927</v>
       </c>
       <c r="B57" s="21">
         <v>9406.9836111111108</v>
@@ -12508,7 +12510,7 @@
     <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" s="48">
         <f t="shared" si="0"/>
-        <v>25966.999988425927</v>
+        <v>25960.999988425927</v>
       </c>
       <c r="B58" s="21">
         <v>9574.9836111111108</v>
@@ -12592,7 +12594,7 @@
     <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59" s="48">
         <f t="shared" si="0"/>
-        <v>25973.999988425927</v>
+        <v>25967.999988425927</v>
       </c>
       <c r="B59" s="21">
         <v>9742.9836111111108</v>
@@ -12676,7 +12678,7 @@
     <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60" s="48">
         <f t="shared" si="0"/>
-        <v>25980.999988425927</v>
+        <v>25974.999988425927</v>
       </c>
       <c r="B60" s="21">
         <v>9910.9836111111108</v>
@@ -12760,7 +12762,7 @@
     <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" s="48">
         <f t="shared" si="0"/>
-        <v>25987.999988425927</v>
+        <v>25981.999988425927</v>
       </c>
       <c r="B61" s="21">
         <v>10078.983611111111</v>
@@ -12844,7 +12846,7 @@
     <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" s="48">
         <f t="shared" si="0"/>
-        <v>25994.999988425927</v>
+        <v>25988.999988425927</v>
       </c>
       <c r="B62" s="21">
         <v>10246.983611111111</v>
@@ -12928,7 +12930,7 @@
     <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63" s="48">
         <f t="shared" si="0"/>
-        <v>26001.999988425927</v>
+        <v>25995.999988425927</v>
       </c>
       <c r="B63" s="21">
         <v>10414.983611111111</v>
@@ -13012,7 +13014,7 @@
     <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64" s="48">
         <f t="shared" si="0"/>
-        <v>26008.999988425927</v>
+        <v>26002.999988425927</v>
       </c>
       <c r="B64" s="21">
         <v>10582.983611111111</v>
@@ -13096,7 +13098,7 @@
     <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65" s="48">
         <f t="shared" si="0"/>
-        <v>26015.999988425927</v>
+        <v>26009.999988425927</v>
       </c>
       <c r="B65" s="21">
         <v>10750.983611111111</v>
@@ -13180,7 +13182,7 @@
     <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66" s="48">
         <f t="shared" si="0"/>
-        <v>26022.999988425927</v>
+        <v>26016.999988425927</v>
       </c>
       <c r="B66" s="21">
         <v>10918.983611111111</v>
@@ -13264,7 +13266,7 @@
     <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67" s="48">
         <f t="shared" si="0"/>
-        <v>26029.999988425927</v>
+        <v>26023.999988425927</v>
       </c>
       <c r="B67" s="21">
         <v>11086.983611111111</v>
@@ -13348,7 +13350,7 @@
     <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68" s="48">
         <f t="shared" ref="A68:A100" si="1">A67+7</f>
-        <v>26036.999988425927</v>
+        <v>26030.999988425927</v>
       </c>
       <c r="B68" s="21">
         <v>11254.983611111111</v>
@@ -13432,7 +13434,7 @@
     <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69" s="48">
         <f t="shared" si="1"/>
-        <v>26043.999988425927</v>
+        <v>26037.999988425927</v>
       </c>
       <c r="B69" s="21">
         <v>11422.983611111111</v>
@@ -13516,7 +13518,7 @@
     <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70" s="48">
         <f t="shared" si="1"/>
-        <v>26050.999988425927</v>
+        <v>26044.999988425927</v>
       </c>
       <c r="B70" s="21">
         <v>11590.983611111111</v>
@@ -13600,7 +13602,7 @@
     <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71" s="48">
         <f t="shared" si="1"/>
-        <v>26057.999988425927</v>
+        <v>26051.999988425927</v>
       </c>
       <c r="B71" s="21">
         <v>11758.983611111111</v>
@@ -13684,7 +13686,7 @@
     <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72" s="48">
         <f t="shared" si="1"/>
-        <v>26064.999988425927</v>
+        <v>26058.999988425927</v>
       </c>
       <c r="B72" s="21">
         <v>11926.983611111111</v>
@@ -13768,7 +13770,7 @@
     <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73" s="48">
         <f t="shared" si="1"/>
-        <v>26071.999988425927</v>
+        <v>26065.999988425927</v>
       </c>
       <c r="B73" s="21">
         <v>12094.983611111111</v>
@@ -13852,7 +13854,7 @@
     <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74" s="48">
         <f t="shared" si="1"/>
-        <v>26078.999988425927</v>
+        <v>26072.999988425927</v>
       </c>
       <c r="B74" s="21">
         <v>12262.983611111111</v>
@@ -13936,7 +13938,7 @@
     <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75" s="48">
         <f t="shared" si="1"/>
-        <v>26085.999988425927</v>
+        <v>26079.999988425927</v>
       </c>
       <c r="B75" s="21">
         <v>12430.983611111111</v>
@@ -14020,7 +14022,7 @@
     <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76" s="48">
         <f t="shared" si="1"/>
-        <v>26092.999988425927</v>
+        <v>26086.999988425927</v>
       </c>
       <c r="B76" s="21">
         <v>12598.983611111111</v>
@@ -14104,7 +14106,7 @@
     <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77" s="48">
         <f t="shared" si="1"/>
-        <v>26099.999988425927</v>
+        <v>26093.999988425927</v>
       </c>
       <c r="B77" s="21">
         <v>12766.983611111111</v>
@@ -14188,7 +14190,7 @@
     <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78" s="48">
         <f t="shared" si="1"/>
-        <v>26106.999988425927</v>
+        <v>26100.999988425927</v>
       </c>
       <c r="B78" s="21">
         <v>12934.983611111111</v>
@@ -14272,7 +14274,7 @@
     <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79" s="48">
         <f t="shared" si="1"/>
-        <v>26113.999988425927</v>
+        <v>26107.999988425927</v>
       </c>
       <c r="B79" s="21">
         <v>13102.983611111111</v>
@@ -14356,7 +14358,7 @@
     <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80" s="48">
         <f t="shared" si="1"/>
-        <v>26120.999988425927</v>
+        <v>26114.999988425927</v>
       </c>
       <c r="B80" s="21">
         <v>13270.983611111111</v>
@@ -14440,7 +14442,7 @@
     <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" s="48">
         <f t="shared" si="1"/>
-        <v>26127.999988425927</v>
+        <v>26121.999988425927</v>
       </c>
       <c r="B81" s="21">
         <v>13438.983611111111</v>
@@ -14524,7 +14526,7 @@
     <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" s="48">
         <f t="shared" si="1"/>
-        <v>26134.999988425927</v>
+        <v>26128.999988425927</v>
       </c>
       <c r="B82" s="21">
         <v>13606.983611111111</v>
@@ -14608,7 +14610,7 @@
     <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" s="48">
         <f t="shared" si="1"/>
-        <v>26141.999988425927</v>
+        <v>26135.999988425927</v>
       </c>
       <c r="B83" s="21">
         <v>13774.983611111111</v>
@@ -14692,7 +14694,7 @@
     <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" s="48">
         <f t="shared" si="1"/>
-        <v>26148.999988425927</v>
+        <v>26142.999988425927</v>
       </c>
       <c r="B84" s="21">
         <v>13942.983611111111</v>
@@ -14776,7 +14778,7 @@
     <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" s="48">
         <f t="shared" si="1"/>
-        <v>26155.999988425927</v>
+        <v>26149.999988425927</v>
       </c>
       <c r="B85" s="21">
         <v>14110.983611111111</v>
@@ -14860,7 +14862,7 @@
     <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86" s="48">
         <f t="shared" si="1"/>
-        <v>26162.999988425927</v>
+        <v>26156.999988425927</v>
       </c>
       <c r="B86" s="21">
         <v>14278.983611111111</v>
@@ -14944,7 +14946,7 @@
     <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87" s="48">
         <f t="shared" si="1"/>
-        <v>26169.999988425927</v>
+        <v>26163.999988425927</v>
       </c>
       <c r="B87" s="21">
         <v>14446.983611111111</v>
@@ -15028,7 +15030,7 @@
     <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" s="48">
         <f t="shared" si="1"/>
-        <v>26176.999988425927</v>
+        <v>26170.999988425927</v>
       </c>
       <c r="B88" s="21">
         <v>14614.983611111111</v>
@@ -15112,7 +15114,7 @@
     <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" s="48">
         <f t="shared" si="1"/>
-        <v>26183.999988425927</v>
+        <v>26177.999988425927</v>
       </c>
       <c r="B89" s="21">
         <v>14782.983611111111</v>
@@ -15196,7 +15198,7 @@
     <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" s="48">
         <f t="shared" si="1"/>
-        <v>26190.999988425927</v>
+        <v>26184.999988425927</v>
       </c>
       <c r="B90" s="21">
         <v>14950.983611111111</v>
@@ -15280,7 +15282,7 @@
     <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91" s="48">
         <f t="shared" si="1"/>
-        <v>26197.999988425927</v>
+        <v>26191.999988425927</v>
       </c>
       <c r="B91" s="21">
         <v>15118.983611111111</v>
@@ -15364,7 +15366,7 @@
     <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92" s="48">
         <f t="shared" si="1"/>
-        <v>26204.999988425927</v>
+        <v>26198.999988425927</v>
       </c>
       <c r="B92" s="21">
         <v>15286.983611111111</v>
@@ -15448,7 +15450,7 @@
     <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93" s="48">
         <f t="shared" si="1"/>
-        <v>26211.999988425927</v>
+        <v>26205.999988425927</v>
       </c>
       <c r="B93" s="21">
         <v>15454.983611111111</v>
@@ -15532,7 +15534,7 @@
     <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94" s="48">
         <f t="shared" si="1"/>
-        <v>26218.999988425927</v>
+        <v>26212.999988425927</v>
       </c>
       <c r="B94" s="21">
         <v>15622.983611111111</v>
@@ -15616,7 +15618,7 @@
     <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" s="48">
         <f t="shared" si="1"/>
-        <v>26225.999988425927</v>
+        <v>26219.999988425927</v>
       </c>
       <c r="B95" s="21">
         <v>15790.983611111111</v>
@@ -15700,7 +15702,7 @@
     <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" s="48">
         <f t="shared" si="1"/>
-        <v>26232.999988425927</v>
+        <v>26226.999988425927</v>
       </c>
       <c r="B96" s="21">
         <v>15958.983611111111</v>
@@ -15784,7 +15786,7 @@
     <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" s="48">
         <f t="shared" si="1"/>
-        <v>26239.999988425927</v>
+        <v>26233.999988425927</v>
       </c>
       <c r="B97" s="21">
         <v>16126.983611111111</v>
@@ -15868,7 +15870,7 @@
     <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" s="48">
         <f t="shared" si="1"/>
-        <v>26246.999988425927</v>
+        <v>26240.999988425927</v>
       </c>
       <c r="B98" s="21">
         <v>16294.983611111111</v>
@@ -15952,7 +15954,7 @@
     <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" s="48">
         <f t="shared" si="1"/>
-        <v>26253.999988425927</v>
+        <v>26247.999988425927</v>
       </c>
       <c r="B99" s="21">
         <v>16462.983611111111</v>
@@ -16036,7 +16038,7 @@
     <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" s="48">
         <f t="shared" si="1"/>
-        <v>26260.999988425927</v>
+        <v>26254.999988425927</v>
       </c>
       <c r="B100" s="21">
         <v>16630.983611111111</v>

</xml_diff>